<commit_message>
Removed unused containers from azure blob storage map excel spreadsheet
</commit_message>
<xml_diff>
--- a/Cloud Storage Maps/Azure Storage/Blob.xlsx
+++ b/Cloud Storage Maps/Azure Storage/Blob.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tihanewi\Downloads\ApexVisual.F1_2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tihanewi\Downloads\ApexVisual.F1_2020\Cloud Storage Maps\Azure Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DFF00F-F999-47EF-9223-2DB76F0D772A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F490F3E0-815E-4AE1-96F9-54F590E0A213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51765" yWindow="2775" windowWidth="16875" windowHeight="10530" xr2:uid="{B8006B69-B989-4F9B-ABBC-61625677C1A0}"/>
+    <workbookView xWindow="47730" yWindow="1155" windowWidth="20475" windowHeight="11415" xr2:uid="{B8006B69-B989-4F9B-ABBC-61625677C1A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Containers" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Container Name</t>
   </si>
@@ -44,21 +44,9 @@
     <t>sessions</t>
   </si>
   <si>
-    <t>sessionsummaries</t>
-  </si>
-  <si>
-    <t>sessionanalyses</t>
-  </si>
-  <si>
     <t>Raw telemetry for a session</t>
   </si>
   <si>
-    <t>A smaller object that descripts the session. For example, the car used, team, what track you were on, what day it was on, etc.</t>
-  </si>
-  <si>
-    <t>A fully converted SessionAnalysis object (generated from a session as seen in the container above)</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -68,18 +56,12 @@
     <t>Users</t>
   </si>
   <si>
-    <t>useraccounts</t>
-  </si>
-  <si>
     <t>Naming Convention</t>
   </si>
   <si>
     <t>userphotos</t>
   </si>
   <si>
-    <t>Contains the JSON object for the user accounts (i.e. username, password, email, and owned session ID's, reference to photo blob ID)</t>
-  </si>
-  <si>
     <t>contains users profile pictures</t>
   </si>
   <si>
@@ -90,9 +72,6 @@
   </si>
   <si>
     <t>The unique session ID</t>
-  </si>
-  <si>
-    <t>The username of the user</t>
   </si>
   <si>
     <t>activitylogs</t>
@@ -486,11 +465,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5C40B7-953D-434C-8823-1D3A499E1342}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -502,7 +479,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -511,46 +488,46 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -558,62 +535,26 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>